<commit_message>
add base result to excel
</commit_message>
<xml_diff>
--- a/practise/final/res/results.xlsx
+++ b/practise/final/res/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcs163\works\git_repos\ADL-MAE\practise\final\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdadf\OneDrive\Documents\GitHub\ADL-MAE\practise\final\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BF2B9D-E21E-49BD-9A13-CE8E3366136A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77D4BC-E9FC-4470-B61D-86E03DECC63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1371ED61-D174-4E49-A7CC-3BA8ABBD767D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1371ED61-D174-4E49-A7CC-3BA8ABBD767D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>mask_ratio</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>n param</t>
+  </si>
+  <si>
+    <t>exp#5 base</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -326,7 +332,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,6 +341,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -761,23 +770,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EFFAC3-6709-4E8F-A586-25C63BC9BC9D}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="17.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="2" max="2" width="17.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -794,8 +804,11 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -814,8 +827,11 @@
       <c r="G2" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
@@ -834,8 +850,11 @@
       <c r="G3" s="2">
         <v>68.33</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -854,8 +873,11 @@
       <c r="G4" s="2">
         <v>95.540999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2">
+        <v>80.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -874,8 +896,11 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -894,8 +919,11 @@
       <c r="G6" s="2">
         <v>0.36413000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="4">
+        <v>3.0329754976999102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -914,8 +942,11 @@
       <c r="G7" s="2">
         <v>0.95679000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="4">
+        <v>1.9656921426455101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -934,8 +965,11 @@
       <c r="G8" s="2">
         <v>1.0077</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="4">
+        <v>1.9396396428346601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
@@ -954,8 +988,11 @@
       <c r="G9" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -974,8 +1011,14 @@
       <c r="G10" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="2">
+        <v>200</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -994,8 +1037,11 @@
       <c r="G11" s="2">
         <v>512</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1014,9 +1060,12 @@
       <c r="G12" s="2">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>